<commit_message>
add questions to qa_algos file
</commit_message>
<xml_diff>
--- a/data/QA_Algorithms.xlsx
+++ b/data/QA_Algorithms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\github_projects\data-science-helper-bot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986E4A7C-1A9F-433C-A479-7BAAC6A3B364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53425CF-DD6A-4AF1-82B2-8742D29C50D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17680" yWindow="0" windowWidth="16720" windowHeight="14400" xr2:uid="{26641EAC-8151-457B-9A4B-828670598D44}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="72">
   <si>
     <t>ответ 1</t>
   </si>
@@ -288,12 +288,51 @@
   <si>
     <t>нельзя упростить</t>
   </si>
+  <si>
+    <t>массив</t>
+  </si>
+  <si>
+    <t>Достоинства статического массива</t>
+  </si>
+  <si>
+    <t>1. Скорость доступа к произвольному элементу O(1) для записи или чтения значения.
+2. Просто реализуется и удобен для небольших наборов данных.</t>
+  </si>
+  <si>
+    <t>Недостатки статического массива:</t>
+  </si>
+  <si>
+    <t>1. Хранение данных выполняется в непрерывной области памяти. Не всегда эффективно для очень больших объемов данных. 
+2. Статический массив не может менять число своих элементов в процессе работы программы. Если зарезервированного места окажется недостаточно, то данные могут потеряться. 
+3. Вставка и удаление элементов выполняется за время O(n). Может быть критично при больших n.</t>
+  </si>
+  <si>
+    <t>Какова вычислительная сложность операции добавления нового значения в конец статического массива размера n (при условии, что места для записи значения в массиве достаточно и мы уже знаем индекс ячейки, куда заносится новое значение)?</t>
+  </si>
+  <si>
+    <t>O(1)</t>
+  </si>
+  <si>
+    <t>Какова вычислительная сложность операции добавления нового значения в начало статического массива размера n (при условии, что места для записи значения в массиве достаточно)?</t>
+  </si>
+  <si>
+    <t>O(n)</t>
+  </si>
+  <si>
+    <t>Какова вычислительная сложность операции вставки нового значения в произвольную позицию статического массива размера n (при условии, что места для записи значения в массиве достаточно)?</t>
+  </si>
+  <si>
+    <t>Какова вычислительная сложность операции удаления последнего значения статического массива размера n?</t>
+  </si>
+  <si>
+    <t> Какова вычислительная сложность операции удаления произвольного значения статического массива размера n?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,20 +345,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Yandex Sans Display Light"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="13.3"/>
-      <color rgb="FF222222"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -342,7 +367,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -352,12 +377,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -673,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69434668-5E94-444C-AE4B-BFC8926C8198}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1079,11 +1098,106 @@
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="17.5">
-      <c r="C30" s="5"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="C32" s="4"/>
+    <row r="29" spans="1:4" ht="43.5">
+      <c r="A29">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="101.5">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="72.5">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="58">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="58">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="29">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="29">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>